<commit_message>
office hours update and email fix
</commit_message>
<xml_diff>
--- a/materials/min_lesson_teams.xlsx
+++ b/materials/min_lesson_teams.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20660" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27360" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -252,9 +252,6 @@
     <t>Jennifer.Weadock@uvm.edu</t>
   </si>
   <si>
-    <t>Mackenzie.T.Young@uvm.edu</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -481,6 +478,9 @@
   </si>
   <si>
     <t>Exponential Functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> myoung14@uvm.edu</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -543,6 +543,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -771,15 +811,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="225">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1337,161 +1384,161 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>42269</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2" t="s">
-        <v>126</v>
+      <c r="F2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="H2" t="s">
+        <v>148</v>
+      </c>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" t="s">
         <v>149</v>
       </c>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="5"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" t="s">
-        <v>121</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="4"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="4"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="9"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="4">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3">
+        <v>42271</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H6" t="s">
         <v>150</v>
       </c>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="5"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G4" t="s">
-        <v>136</v>
-      </c>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="5"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="5">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="4">
-        <v>42271</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" t="s">
-        <v>118</v>
-      </c>
-      <c r="H6" t="s">
-        <v>151</v>
-      </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="5"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" t="s">
-        <v>114</v>
+      <c r="F7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="H7">
         <v>2.2000000000000002</v>
@@ -1499,144 +1546,144 @@
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="5"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="F8" t="s">
-        <v>106</v>
-      </c>
-      <c r="G8" t="s">
-        <v>141</v>
+      <c r="F8" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="5"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="9"/>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>3</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>42276</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F10" t="s">
-        <v>113</v>
-      </c>
-      <c r="G10" t="s">
-        <v>148</v>
+      <c r="F10" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>147</v>
       </c>
       <c r="H10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="5"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F11" t="s">
-        <v>87</v>
-      </c>
-      <c r="G11" t="s">
-        <v>122</v>
+      <c r="F11" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="H11">
         <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="5"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="4">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3">
+        <v>42278</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H14" t="s">
+        <v>152</v>
+      </c>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="4"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G15" s="8" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="5"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="5">
-        <v>4</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="4">
-        <v>42278</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" t="s">
-        <v>88</v>
-      </c>
-      <c r="G14" t="s">
-        <v>123</v>
-      </c>
-      <c r="H14" t="s">
-        <v>153</v>
-      </c>
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="5"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" t="s">
-        <v>90</v>
-      </c>
-      <c r="G15" t="s">
-        <v>125</v>
       </c>
       <c r="H15">
         <v>2.4</v>
@@ -1644,659 +1691,659 @@
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="5"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" t="s">
+      <c r="A16" s="4"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="8" t="s">
         <v>64</v>
       </c>
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="5"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>5</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>42283</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="4"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="4"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="4"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="4">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3">
+        <v>42285</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="4"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="4"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="4"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="4">
+        <v>7</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3">
+        <v>42290</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="4"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="4"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="4"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="4">
+        <v>8</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="3">
+        <v>42292</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="4"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="4"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="4"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="4">
+        <v>9</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="3">
+        <v>42297</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="4"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="4"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="4"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="4">
+        <v>10</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="3">
+        <v>42299</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="4"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="4"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="4"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="4">
+        <v>11</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="3">
+        <v>42304</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G42" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="5"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" t="s">
-        <v>109</v>
-      </c>
-      <c r="G19" t="s">
-        <v>144</v>
-      </c>
-      <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="5"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" t="s">
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="4"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="4"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="4"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="4">
+        <v>12</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="3">
+        <v>42306</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="4"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="4"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="4"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="4">
+        <v>13</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="3">
+        <v>42311</v>
+      </c>
+      <c r="D50" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F20" t="s">
-        <v>97</v>
-      </c>
-      <c r="G20" t="s">
-        <v>132</v>
-      </c>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="5"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="5">
-        <v>6</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="E50" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="4"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="4"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="4"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="4">
+        <v>14</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="4">
-        <v>42285</v>
-      </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F22" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="5"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23" t="s">
-        <v>95</v>
-      </c>
-      <c r="G23" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="5"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" t="s">
-        <v>104</v>
-      </c>
-      <c r="G24" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="5"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="5">
-        <v>7</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="C54" s="3">
+        <v>42313</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="4">
-        <v>42290</v>
-      </c>
-      <c r="D26" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" t="s">
-        <v>99</v>
-      </c>
-      <c r="G26" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="5"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" t="s">
-        <v>100</v>
-      </c>
-      <c r="G27" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="5"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" t="s">
-        <v>112</v>
-      </c>
-      <c r="G28" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="5"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="5">
-        <v>8</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="C58" s="3">
+        <v>42318</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="4">
-        <v>42292</v>
-      </c>
-      <c r="D30" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" t="s">
-        <v>74</v>
-      </c>
-      <c r="F30" t="s">
-        <v>105</v>
-      </c>
-      <c r="G30" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="5"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" t="s">
-        <v>111</v>
-      </c>
-      <c r="G31" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="5"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" t="s">
-        <v>72</v>
-      </c>
-      <c r="F32" t="s">
-        <v>110</v>
-      </c>
-      <c r="G32" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="5"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="5">
-        <v>9</v>
-      </c>
-      <c r="B34" s="3" t="s">
+      <c r="C62" s="3">
+        <v>42320</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="4">
-        <v>42297</v>
-      </c>
-      <c r="D34" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" t="s">
-        <v>75</v>
-      </c>
-      <c r="F34" t="s">
-        <v>98</v>
-      </c>
-      <c r="G34" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="5"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" t="s">
-        <v>33</v>
-      </c>
-      <c r="E35" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" t="s">
-        <v>107</v>
-      </c>
-      <c r="G35" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="5"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" t="s">
-        <v>71</v>
-      </c>
-      <c r="F36" t="s">
-        <v>108</v>
-      </c>
-      <c r="G36" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="5"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="5">
-        <v>10</v>
-      </c>
-      <c r="B38" s="3" t="s">
+      <c r="C66" s="3">
+        <v>42325</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="4">
-        <v>42299</v>
-      </c>
-      <c r="D38" t="s">
-        <v>37</v>
-      </c>
-      <c r="E38" t="s">
-        <v>46</v>
-      </c>
-      <c r="F38" t="s">
-        <v>102</v>
-      </c>
-      <c r="G38" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="5"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" t="s">
-        <v>65</v>
-      </c>
-      <c r="F39" t="s">
-        <v>103</v>
-      </c>
-      <c r="G39" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="5"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" t="s">
-        <v>26</v>
-      </c>
-      <c r="E40" t="s">
-        <v>57</v>
-      </c>
-      <c r="F40" t="s">
-        <v>94</v>
-      </c>
-      <c r="G40" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="5"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="5">
-        <v>11</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" s="4">
-        <v>42304</v>
-      </c>
-      <c r="D42" t="s">
-        <v>36</v>
-      </c>
-      <c r="E42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F42" t="s">
-        <v>93</v>
-      </c>
-      <c r="G42" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="5"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F43" t="s">
-        <v>85</v>
-      </c>
-      <c r="G43" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="5"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" t="s">
-        <v>31</v>
-      </c>
-      <c r="E44" t="s">
-        <v>52</v>
-      </c>
-      <c r="F44" t="s">
-        <v>84</v>
-      </c>
-      <c r="G44" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="5"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="5">
-        <v>12</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="4">
-        <v>42306</v>
-      </c>
-      <c r="D46" t="s">
-        <v>35</v>
-      </c>
-      <c r="E46" t="s">
-        <v>48</v>
-      </c>
-      <c r="F46" t="s">
-        <v>82</v>
-      </c>
-      <c r="G46" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="5"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" t="s">
-        <v>34</v>
-      </c>
-      <c r="E47" t="s">
-        <v>49</v>
-      </c>
-      <c r="F47" t="s">
-        <v>81</v>
-      </c>
-      <c r="G47" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="5"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" t="s">
-        <v>29</v>
-      </c>
-      <c r="E48" t="s">
-        <v>54</v>
-      </c>
-      <c r="F48" t="s">
-        <v>80</v>
-      </c>
-      <c r="G48" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="5"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="5">
-        <v>13</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C50" s="4">
-        <v>42311</v>
-      </c>
-      <c r="D50" t="s">
-        <v>78</v>
-      </c>
-      <c r="E50" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="5"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="5"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="5"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="5">
-        <v>14</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C54" s="4">
-        <v>42313</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C58" s="4">
-        <v>42318</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62" s="4">
-        <v>42320</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C66" s="4">
-        <v>42325</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="3"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C70" s="4">
+      <c r="C70" s="3">
         <v>42327</v>
       </c>
     </row>

</xml_diff>

<commit_message>
quiz2 mistakes added and minilesson updates
</commit_message>
<xml_diff>
--- a/materials/min_lesson_teams.xlsx
+++ b/materials/min_lesson_teams.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27360" windowHeight="17540" tabRatio="500"/>
   </bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="162">
   <si>
     <t>Date</t>
   </si>
@@ -249,9 +249,6 @@
     <t>Jennifer.Weadock@uvm.edu</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Albee, May V.</t>
   </si>
   <si>
@@ -481,6 +478,33 @@
   </si>
   <si>
     <t>askahen@uvm.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logarithms </t>
+  </si>
+  <si>
+    <t>Limits</t>
+  </si>
+  <si>
+    <t>Test Day</t>
+  </si>
+  <si>
+    <t>Continuity</t>
+  </si>
+  <si>
+    <t>Rate of Change</t>
+  </si>
+  <si>
+    <t>The Derivative</t>
+  </si>
+  <si>
+    <t>Finding Derivatives</t>
+  </si>
+  <si>
+    <t>Product Rule</t>
+  </si>
+  <si>
+    <t>Chain Rule</t>
   </si>
 </sst>
 </file>
@@ -584,7 +608,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="225">
+  <cellStyleXfs count="233">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -810,8 +834,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -827,8 +859,9 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="225">
+  <cellStyles count="233">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -941,6 +974,10 @@
     <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1053,6 +1090,10 @@
     <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1385,7 +1426,7 @@
   <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1439,13 +1480,13 @@
         <v>51</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K2" s="1"/>
     </row>
@@ -1460,13 +1501,13 @@
         <v>68</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -1481,10 +1522,10 @@
         <v>59</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -1514,13 +1555,13 @@
         <v>73</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K6" s="1"/>
     </row>
@@ -1535,10 +1576,10 @@
         <v>63</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H7">
         <v>2.2000000000000002</v>
@@ -1556,10 +1597,10 @@
         <v>53</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K8" s="1"/>
     </row>
@@ -1589,13 +1630,13 @@
         <v>43</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K10" s="1"/>
     </row>
@@ -1610,10 +1651,10 @@
         <v>56</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H11">
         <v>2.2999999999999998</v>
@@ -1630,10 +1671,10 @@
         <v>55</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1659,13 +1700,13 @@
         <v>58</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K14" s="1"/>
     </row>
@@ -1680,10 +1721,10 @@
         <v>61</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H15">
         <v>2.4</v>
@@ -1725,10 +1766,13 @@
         <v>62</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>153</v>
       </c>
       <c r="K18" s="1"/>
     </row>
@@ -1743,10 +1787,13 @@
         <v>60</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
+      </c>
+      <c r="H19">
+        <v>2.5</v>
       </c>
       <c r="K19" s="1"/>
     </row>
@@ -1758,13 +1805,13 @@
         <v>6</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K20" s="1"/>
     </row>
@@ -1775,70 +1822,31 @@
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="4">
-        <v>6</v>
-      </c>
       <c r="B22" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="3">
         <v>42285</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>129</v>
+      <c r="H22" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="4"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>128</v>
-      </c>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="4"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>137</v>
-      </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="4"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>2</v>
@@ -1847,16 +1855,19 @@
         <v>42290</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1864,16 +1875,19 @@
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>133</v>
+        <v>127</v>
+      </c>
+      <c r="H27">
+        <v>3.1</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1881,16 +1895,16 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1900,7 +1914,7 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>3</v>
@@ -1909,16 +1923,19 @@
         <v>42292</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>153</v>
+        <v>44</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>138</v>
+        <v>131</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1926,16 +1943,19 @@
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="7" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>144</v>
+        <v>132</v>
+      </c>
+      <c r="H31">
+        <v>3.2</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1943,26 +1963,26 @@
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="4"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:8">
       <c r="A34" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>2</v>
@@ -1971,60 +1991,66 @@
         <v>42297</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>74</v>
+        <v>152</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>137</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="4"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>143</v>
+      </c>
+      <c r="H35">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="4"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="4"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:8">
       <c r="A38" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>3</v>
@@ -2033,60 +2059,66 @@
         <v>42299</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>130</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="4"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="7" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>139</v>
+      </c>
+      <c r="H39">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="4"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="7" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="4"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:8">
       <c r="A42" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>2</v>
@@ -2095,60 +2127,66 @@
         <v>42304</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>134</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="4"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>54</v>
+      <c r="D43" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>135</v>
+      </c>
+      <c r="H43">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="4"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="4"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:8">
       <c r="A46" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>3</v>
@@ -2157,60 +2195,66 @@
         <v>42306</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>125</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="4"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>49</v>
+      <c r="D47" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>117</v>
+      </c>
+      <c r="H47">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="4"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="4"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:8">
       <c r="A50" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>2</v>
@@ -2219,30 +2263,66 @@
         <v>42311</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>48</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="4"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="D51" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H51">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="4"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="D52" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" s="4"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:8">
       <c r="A54" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>3</v>
@@ -2251,23 +2331,25 @@
         <v>42313</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="2"/>
+    <row r="55" spans="1:8">
+      <c r="A55" s="4"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
     </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="2"/>
+    <row r="56" spans="1:8">
+      <c r="A56" s="4"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
     </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="2"/>
+    <row r="57" spans="1:8">
+      <c r="A57" s="4"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="2"/>
+    <row r="58" spans="1:8">
+      <c r="A58" s="4">
+        <v>14</v>
+      </c>
       <c r="B58" s="2" t="s">
         <v>2</v>
       </c>
@@ -2275,22 +2357,22 @@
         <v>42318</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:8">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:8">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:8">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:8">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
         <v>3</v>
@@ -2299,12 +2381,12 @@
         <v>42320</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:8">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:8">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>

</xml_diff>